<commit_message>
test results for sciama model
</commit_message>
<xml_diff>
--- a/code/test results.xlsx
+++ b/code/test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1077B23-BD73-47D1-BA4D-1462B91A8FFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB3AE59-022E-4F0B-9145-D8891A78812B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-28800" yWindow="5400" windowWidth="28800" windowHeight="15435" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="135">
   <si>
     <t>test number</t>
   </si>
@@ -487,6 +487,24 @@
   </si>
   <si>
     <t>best_model_061.pth</t>
+  </si>
+  <si>
+    <t>500 (66)</t>
+  </si>
+  <si>
+    <t>best_model_062.pth</t>
+  </si>
+  <si>
+    <t>500 (39)</t>
+  </si>
+  <si>
+    <t>best_model_063.pth</t>
+  </si>
+  <si>
+    <t>best_model_064.pth</t>
+  </si>
+  <si>
+    <t>best_model_065.pth</t>
   </si>
 </sst>
 </file>
@@ -567,7 +585,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -605,20 +623,26 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="38">
     <dxf>
       <fill>
         <patternFill>
@@ -639,9 +663,6 @@
           <bgColor rgb="FF00B050"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -665,7 +686,25 @@
       </fill>
     </dxf>
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -858,6 +897,12 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -936,39 +981,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA105" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A2:AA105" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA109" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A2:AA109" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="50"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:AA76">
     <sortCondition ref="C2:C80"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="30"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="29"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="25"/>
-    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="3"/>
-    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="24"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="23"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="22"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="21"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="20"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="19"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="18"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="17"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="16"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="15"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="14"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="13"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="12"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="11"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="10"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="8"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="35"/>
+    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="33"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="28"/>
+    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="27"/>
+    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1271,10 +1322,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:AA105"/>
+  <dimension ref="A1:AA109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H94" workbookViewId="0">
-      <selection activeCell="N106" sqref="N106"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z109" sqref="Z109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1308,29 +1359,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="S1" s="13" t="s">
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="S1" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1415,7 +1466,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1496,7 +1547,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1577,7 +1628,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1658,7 +1709,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1739,7 +1790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1820,7 +1871,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1901,7 +1952,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1982,7 +2033,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2063,7 +2114,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2144,7 +2195,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2225,7 +2276,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2306,7 +2357,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2387,7 +2438,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2468,7 +2519,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2549,7 +2600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2630,7 +2681,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -2711,7 +2762,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -2792,7 +2843,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -2873,7 +2924,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -2954,7 +3005,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -3035,7 +3086,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -3116,7 +3167,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -3197,7 +3248,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -3278,7 +3329,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -3359,7 +3410,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -3440,7 +3491,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -3521,7 +3572,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -3602,7 +3653,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -3683,7 +3734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -3764,7 +3815,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -3845,7 +3896,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -3926,7 +3977,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -4007,7 +4058,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -4090,7 +4141,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -4171,7 +4222,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -4252,7 +4303,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -4333,7 +4384,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -4414,7 +4465,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -4495,7 +4546,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -4576,7 +4627,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -4659,7 +4710,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -4742,7 +4793,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -4825,7 +4876,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41</v>
       </c>
@@ -4906,7 +4957,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -4989,7 +5040,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -5072,7 +5123,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -5153,7 +5204,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -5234,7 +5285,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -5315,7 +5366,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -5396,7 +5447,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -5477,7 +5528,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -5558,7 +5609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -5639,7 +5690,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -5720,7 +5771,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -5803,7 +5854,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -5886,7 +5937,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -5967,7 +6018,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -6048,7 +6099,7 @@
       </c>
       <c r="AA59" s="2"/>
     </row>
-    <row r="60" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -6127,7 +6178,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="2"/>
     </row>
-    <row r="61" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -6206,7 +6257,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="2"/>
     </row>
-    <row r="62" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -6285,7 +6336,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="2"/>
     </row>
-    <row r="63" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -6364,7 +6415,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="2"/>
     </row>
-    <row r="64" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -6447,7 +6498,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -6528,7 +6579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -7338,7 +7389,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -7419,7 +7470,7 @@
       </c>
       <c r="AA76" s="2"/>
     </row>
-    <row r="77" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -7581,7 +7632,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -7662,7 +7713,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -7743,7 +7794,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="60" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -7826,7 +7877,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -7907,7 +7958,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -7990,7 +8041,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -8071,7 +8122,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -8152,7 +8203,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -8233,7 +8284,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -8316,7 +8367,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -8399,7 +8450,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -8480,7 +8531,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -9128,7 +9179,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>94</v>
       </c>
@@ -9209,7 +9260,7 @@
       </c>
       <c r="AA98" s="2"/>
     </row>
-    <row r="99" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>95</v>
       </c>
@@ -9290,7 +9341,7 @@
       </c>
       <c r="AA99" s="2"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>96</v>
       </c>
@@ -9366,10 +9417,10 @@
       <c r="Y100" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Z100" s="14"/>
+      <c r="Z100" s="13"/>
       <c r="AA100" s="2"/>
     </row>
-    <row r="101" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>97</v>
       </c>
@@ -9445,10 +9496,10 @@
       <c r="Y101" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Z101" s="14"/>
+      <c r="Z101" s="13"/>
       <c r="AA101" s="2"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>98</v>
       </c>
@@ -9524,7 +9575,7 @@
       <c r="Y102" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Z102" s="15"/>
+      <c r="Z102" s="1"/>
       <c r="AA102" s="2"/>
     </row>
     <row r="103" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
@@ -9555,8 +9606,8 @@
       <c r="I103" s="1">
         <v>0.2</v>
       </c>
-      <c r="J103" s="1" t="s">
-        <v>29</v>
+      <c r="J103" s="1">
+        <v>5</v>
       </c>
       <c r="K103" s="1">
         <v>0.2</v>
@@ -9603,7 +9654,7 @@
       <c r="Y103" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Z103" s="1"/>
+      <c r="Z103" s="15"/>
       <c r="AA103" s="2" t="s">
         <v>120</v>
       </c>
@@ -9636,8 +9687,8 @@
       <c r="I104" s="1">
         <v>0.2</v>
       </c>
-      <c r="J104" s="1" t="s">
-        <v>29</v>
+      <c r="J104" s="1">
+        <v>5</v>
       </c>
       <c r="K104" s="1">
         <v>0.2</v>
@@ -9707,7 +9758,7 @@
       <c r="E105" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F105" s="15">
+      <c r="F105" s="1">
         <v>2</v>
       </c>
       <c r="G105" s="1">
@@ -9728,7 +9779,7 @@
       <c r="L105" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M105" s="15">
+      <c r="M105" s="1">
         <v>26800</v>
       </c>
       <c r="N105" s="4" t="s">
@@ -9746,7 +9797,7 @@
       <c r="R105" s="1">
         <v>0</v>
       </c>
-      <c r="S105" s="15">
+      <c r="S105" s="1">
         <v>0</v>
       </c>
       <c r="T105" s="4">
@@ -9770,6 +9821,330 @@
       <c r="Z105" s="1"/>
       <c r="AA105" s="2" t="s">
         <v>128</v>
+      </c>
+    </row>
+    <row r="106" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
+        <v>102</v>
+      </c>
+      <c r="B106" s="1">
+        <v>2</v>
+      </c>
+      <c r="C106" s="15">
+        <v>50</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F106" s="15">
+        <v>2</v>
+      </c>
+      <c r="G106" s="1">
+        <v>0</v>
+      </c>
+      <c r="H106" s="15">
+        <v>0</v>
+      </c>
+      <c r="I106" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J106" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K106" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="L106" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M106" s="15">
+        <v>26800</v>
+      </c>
+      <c r="N106" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="O106" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P106" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q106" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="R106" s="15">
+        <v>0</v>
+      </c>
+      <c r="S106" s="15">
+        <v>0</v>
+      </c>
+      <c r="T106" s="15">
+        <v>128</v>
+      </c>
+      <c r="U106" s="2">
+        <v>97.77</v>
+      </c>
+      <c r="V106" s="2">
+        <v>63</v>
+      </c>
+      <c r="W106" s="2">
+        <v>59</v>
+      </c>
+      <c r="X106" s="7">
+        <v>0.80389999999999995</v>
+      </c>
+      <c r="Y106" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z106" s="1"/>
+      <c r="AA106" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="107" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
+        <v>103</v>
+      </c>
+      <c r="B107" s="1">
+        <v>2</v>
+      </c>
+      <c r="C107" s="15">
+        <v>50</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F107" s="15">
+        <v>2</v>
+      </c>
+      <c r="G107" s="1">
+        <v>0</v>
+      </c>
+      <c r="H107" s="15">
+        <v>0</v>
+      </c>
+      <c r="I107" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K107" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="L107" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M107" s="15">
+        <v>26800</v>
+      </c>
+      <c r="N107" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="O107" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P107" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q107" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="R107" s="15">
+        <v>0</v>
+      </c>
+      <c r="S107" s="15">
+        <v>0</v>
+      </c>
+      <c r="T107" s="4">
+        <v>512</v>
+      </c>
+      <c r="U107" s="2">
+        <v>99.03</v>
+      </c>
+      <c r="V107" s="2">
+        <v>68.13</v>
+      </c>
+      <c r="W107" s="2">
+        <v>26</v>
+      </c>
+      <c r="X107" s="7">
+        <v>0.83360000000000001</v>
+      </c>
+      <c r="Y107" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z107" s="1"/>
+      <c r="AA107" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="108" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A108" s="16">
+        <v>104</v>
+      </c>
+      <c r="B108" s="1">
+        <v>2</v>
+      </c>
+      <c r="C108" s="15">
+        <v>50</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F108" s="15">
+        <v>2</v>
+      </c>
+      <c r="G108" s="1">
+        <v>0</v>
+      </c>
+      <c r="H108" s="15">
+        <v>0</v>
+      </c>
+      <c r="I108" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K108" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="L108" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M108" s="15">
+        <v>26800</v>
+      </c>
+      <c r="N108" s="4">
+        <v>500</v>
+      </c>
+      <c r="O108" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P108" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q108" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="R108" s="15">
+        <v>0</v>
+      </c>
+      <c r="S108" s="15">
+        <v>0</v>
+      </c>
+      <c r="T108" s="15">
+        <v>512</v>
+      </c>
+      <c r="U108" s="2">
+        <v>99.44</v>
+      </c>
+      <c r="V108" s="2">
+        <v>68.150000000000006</v>
+      </c>
+      <c r="W108" s="2">
+        <v>330</v>
+      </c>
+      <c r="X108" s="7">
+        <v>0.82310000000000005</v>
+      </c>
+      <c r="Y108" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z108" s="1"/>
+      <c r="AA108" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>105</v>
+      </c>
+      <c r="B109" s="1">
+        <v>2</v>
+      </c>
+      <c r="C109" s="15">
+        <v>50</v>
+      </c>
+      <c r="D109" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E109" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="F109" s="15">
+        <v>2</v>
+      </c>
+      <c r="G109" s="1">
+        <v>0</v>
+      </c>
+      <c r="H109" s="15">
+        <v>0</v>
+      </c>
+      <c r="I109" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K109" s="15">
+        <v>0.2</v>
+      </c>
+      <c r="L109" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M109" s="15">
+        <v>26800</v>
+      </c>
+      <c r="N109" s="15">
+        <v>500</v>
+      </c>
+      <c r="O109" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="P109" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q109" s="15">
+        <v>1E-3</v>
+      </c>
+      <c r="R109" s="15">
+        <v>0</v>
+      </c>
+      <c r="S109" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="T109" s="15">
+        <v>512</v>
+      </c>
+      <c r="U109" s="2">
+        <v>91.14</v>
+      </c>
+      <c r="V109" s="2">
+        <v>75.650000000000006</v>
+      </c>
+      <c r="W109" s="2">
+        <v>335</v>
+      </c>
+      <c r="X109" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="Y109" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z109" s="1"/>
+      <c r="AA109" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -9778,16 +10153,16 @@
     <mergeCell ref="S1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="U2:U105">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="between">
+  <conditionalFormatting sqref="U2:U109">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
sciama test results on 200 classes
</commit_message>
<xml_diff>
--- a/code/test results.xlsx
+++ b/code/test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB3AE59-022E-4F0B-9145-D8891A78812B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73719973-0A2B-4900-9CE8-8A6D739A0FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5400" windowWidth="28800" windowHeight="15435" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1078" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="139">
   <si>
     <t>test number</t>
   </si>
@@ -505,6 +505,19 @@
   </si>
   <si>
     <t>best_model_065.pth</t>
+  </si>
+  <si>
+    <t>best_model_066.pth</t>
+  </si>
+  <si>
+    <t>best_model_067.pth</t>
+  </si>
+  <si>
+    <t>best_model_068.pth</t>
+  </si>
+  <si>
+    <t>changed code to be more memory efficient
+should NOT cause memory leaks*</t>
   </si>
 </sst>
 </file>
@@ -585,7 +598,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -626,44 +639,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="35">
     <dxf>
       <fill>
         <patternFill>
@@ -981,45 +970,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA109" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
-  <autoFilter ref="A2:AA109" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="50"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA113" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+  <autoFilter ref="A2:AA113" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:AA76">
     <sortCondition ref="C2:C80"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="35"/>
-    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="33"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="32"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="30"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="28"/>
-    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="27"/>
-    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="26"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="32"/>
+    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="30"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="29"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="27"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="26"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="25"/>
+    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="24"/>
+    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="23"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="22"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="20"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="19"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="18"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="17"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="16"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="15"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="14"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="13"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="12"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="11"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="10"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="9"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="7"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1322,10 +1305,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:AA109"/>
+  <dimension ref="A1:AA113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Z109" sqref="Z109"/>
+    <sheetView tabSelected="1" topLeftCell="G85" workbookViewId="0">
+      <selection activeCell="M119" sqref="M119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,29 +1342,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="S1" s="14" t="s">
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="S1" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
@@ -1466,7 +1449,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1547,7 +1530,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1628,7 +1611,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1709,7 +1692,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1790,7 +1773,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1871,7 +1854,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1952,7 +1935,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -2033,7 +2016,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2114,7 +2097,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2195,7 +2178,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2276,7 +2259,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2357,7 +2340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2438,7 +2421,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2519,7 +2502,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2600,7 +2583,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2681,7 +2664,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="18" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -2762,7 +2745,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="19" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -2843,7 +2826,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>16</v>
       </c>
@@ -2924,7 +2907,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="21" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>17</v>
       </c>
@@ -3005,7 +2988,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>18</v>
       </c>
@@ -3086,7 +3069,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>19</v>
       </c>
@@ -3167,7 +3150,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="24" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>20</v>
       </c>
@@ -3248,7 +3231,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>21</v>
       </c>
@@ -3329,7 +3312,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>22</v>
       </c>
@@ -3410,7 +3393,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>23</v>
       </c>
@@ -3491,7 +3474,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>24</v>
       </c>
@@ -3572,7 +3555,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>25</v>
       </c>
@@ -3653,7 +3636,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="30" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>26</v>
       </c>
@@ -3734,7 +3717,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>27</v>
       </c>
@@ -3815,7 +3798,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>28</v>
       </c>
@@ -3896,7 +3879,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>29</v>
       </c>
@@ -3977,7 +3960,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="34" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>30</v>
       </c>
@@ -4058,7 +4041,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="35" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>31</v>
       </c>
@@ -4141,7 +4124,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>32</v>
       </c>
@@ -4222,7 +4205,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>33</v>
       </c>
@@ -4303,7 +4286,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="38" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>34</v>
       </c>
@@ -4384,7 +4367,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="39" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>35</v>
       </c>
@@ -4465,7 +4448,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>36</v>
       </c>
@@ -4546,7 +4529,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="41" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>37</v>
       </c>
@@ -4627,7 +4610,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="42" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>38</v>
       </c>
@@ -4710,7 +4693,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>39</v>
       </c>
@@ -4793,7 +4776,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="44" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>40</v>
       </c>
@@ -4876,7 +4859,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>41</v>
       </c>
@@ -4957,7 +4940,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="46" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>42</v>
       </c>
@@ -5040,7 +5023,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="47" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43</v>
       </c>
@@ -5123,7 +5106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>44</v>
       </c>
@@ -5204,7 +5187,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="49" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -5285,7 +5268,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="50" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>46</v>
       </c>
@@ -5366,7 +5349,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="51" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>47</v>
       </c>
@@ -5447,7 +5430,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="52" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>48</v>
       </c>
@@ -5528,7 +5511,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="53" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>49</v>
       </c>
@@ -5609,7 +5592,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="54" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>50</v>
       </c>
@@ -5690,7 +5673,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>51</v>
       </c>
@@ -5771,7 +5754,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="56" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>52</v>
       </c>
@@ -5854,7 +5837,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="57" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>53</v>
       </c>
@@ -5937,7 +5920,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>54</v>
       </c>
@@ -6018,7 +6001,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>55</v>
       </c>
@@ -6099,7 +6082,7 @@
       </c>
       <c r="AA59" s="2"/>
     </row>
-    <row r="60" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>56</v>
       </c>
@@ -6178,7 +6161,7 @@
       <c r="Z60" s="1"/>
       <c r="AA60" s="2"/>
     </row>
-    <row r="61" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>57</v>
       </c>
@@ -6257,7 +6240,7 @@
       <c r="Z61" s="1"/>
       <c r="AA61" s="2"/>
     </row>
-    <row r="62" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>58</v>
       </c>
@@ -6336,7 +6319,7 @@
       <c r="Z62" s="1"/>
       <c r="AA62" s="2"/>
     </row>
-    <row r="63" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>59</v>
       </c>
@@ -6415,7 +6398,7 @@
       <c r="Z63" s="1"/>
       <c r="AA63" s="2"/>
     </row>
-    <row r="64" spans="1:27" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>60</v>
       </c>
@@ -6498,7 +6481,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>61</v>
       </c>
@@ -6579,7 +6562,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="66" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>62</v>
       </c>
@@ -7389,7 +7372,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:27" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>72</v>
       </c>
@@ -7470,7 +7453,7 @@
       </c>
       <c r="AA76" s="2"/>
     </row>
-    <row r="77" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>73</v>
       </c>
@@ -7632,7 +7615,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="79" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>75</v>
       </c>
@@ -7713,7 +7696,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>76</v>
       </c>
@@ -7794,7 +7777,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:27" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:27" ht="60" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>77</v>
       </c>
@@ -7877,7 +7860,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="82" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>78</v>
       </c>
@@ -7958,7 +7941,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="1:27" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:27" ht="30" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>79</v>
       </c>
@@ -8041,7 +8024,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="84" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>80</v>
       </c>
@@ -8122,7 +8105,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="85" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>81</v>
       </c>
@@ -8203,7 +8186,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="86" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>82</v>
       </c>
@@ -8284,7 +8267,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>83</v>
       </c>
@@ -8367,7 +8350,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="88" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>84</v>
       </c>
@@ -8450,7 +8433,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="89" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>85</v>
       </c>
@@ -8531,7 +8514,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="90" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>86</v>
       </c>
@@ -9179,7 +9162,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="98" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>94</v>
       </c>
@@ -9260,7 +9243,7 @@
       </c>
       <c r="AA98" s="2"/>
     </row>
-    <row r="99" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>95</v>
       </c>
@@ -9341,7 +9324,7 @@
       </c>
       <c r="AA99" s="2"/>
     </row>
-    <row r="100" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>96</v>
       </c>
@@ -9420,7 +9403,7 @@
       <c r="Z100" s="13"/>
       <c r="AA100" s="2"/>
     </row>
-    <row r="101" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>97</v>
       </c>
@@ -9499,7 +9482,7 @@
       <c r="Z101" s="13"/>
       <c r="AA101" s="2"/>
     </row>
-    <row r="102" spans="1:27" ht="15.75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>98</v>
       </c>
@@ -9654,7 +9637,7 @@
       <c r="Y103" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Z103" s="15"/>
+      <c r="Z103" s="1"/>
       <c r="AA103" s="2" t="s">
         <v>120</v>
       </c>
@@ -9830,7 +9813,7 @@
       <c r="B106" s="1">
         <v>2</v>
       </c>
-      <c r="C106" s="15">
+      <c r="C106" s="1">
         <v>50</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -9839,13 +9822,13 @@
       <c r="E106" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F106" s="15">
+      <c r="F106" s="1">
         <v>2</v>
       </c>
       <c r="G106" s="1">
         <v>0</v>
       </c>
-      <c r="H106" s="15">
+      <c r="H106" s="1">
         <v>0</v>
       </c>
       <c r="I106" s="1">
@@ -9854,34 +9837,34 @@
       <c r="J106" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K106" s="15">
+      <c r="K106" s="1">
         <v>0.2</v>
       </c>
       <c r="L106" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M106" s="15">
+      <c r="M106" s="1">
         <v>26800</v>
       </c>
       <c r="N106" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="O106" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P106" s="15" t="s">
+      <c r="O106" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P106" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q106" s="15">
+      <c r="Q106" s="1">
         <v>1E-3</v>
       </c>
-      <c r="R106" s="15">
-        <v>0</v>
-      </c>
-      <c r="S106" s="15">
-        <v>0</v>
-      </c>
-      <c r="T106" s="15">
+      <c r="R106" s="1">
+        <v>0</v>
+      </c>
+      <c r="S106" s="1">
+        <v>0</v>
+      </c>
+      <c r="T106" s="1">
         <v>128</v>
       </c>
       <c r="U106" s="2">
@@ -9911,7 +9894,7 @@
       <c r="B107" s="1">
         <v>2</v>
       </c>
-      <c r="C107" s="15">
+      <c r="C107" s="1">
         <v>50</v>
       </c>
       <c r="D107" s="1" t="s">
@@ -9920,13 +9903,13 @@
       <c r="E107" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F107" s="15">
+      <c r="F107" s="1">
         <v>2</v>
       </c>
       <c r="G107" s="1">
         <v>0</v>
       </c>
-      <c r="H107" s="15">
+      <c r="H107" s="1">
         <v>0</v>
       </c>
       <c r="I107" s="1">
@@ -9935,31 +9918,31 @@
       <c r="J107" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K107" s="15">
+      <c r="K107" s="1">
         <v>0.2</v>
       </c>
       <c r="L107" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M107" s="15">
+      <c r="M107" s="1">
         <v>26800</v>
       </c>
       <c r="N107" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="O107" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P107" s="15" t="s">
+      <c r="O107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P107" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q107" s="15">
+      <c r="Q107" s="1">
         <v>1E-3</v>
       </c>
-      <c r="R107" s="15">
-        <v>0</v>
-      </c>
-      <c r="S107" s="15">
+      <c r="R107" s="1">
+        <v>0</v>
+      </c>
+      <c r="S107" s="1">
         <v>0</v>
       </c>
       <c r="T107" s="4">
@@ -9986,13 +9969,13 @@
       </c>
     </row>
     <row r="108" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A108" s="16">
+      <c r="A108" s="1">
         <v>104</v>
       </c>
       <c r="B108" s="1">
         <v>2</v>
       </c>
-      <c r="C108" s="15">
+      <c r="C108" s="1">
         <v>50</v>
       </c>
       <c r="D108" s="1" t="s">
@@ -10001,13 +9984,13 @@
       <c r="E108" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F108" s="15">
+      <c r="F108" s="1">
         <v>2</v>
       </c>
       <c r="G108" s="1">
         <v>0</v>
       </c>
-      <c r="H108" s="15">
+      <c r="H108" s="1">
         <v>0</v>
       </c>
       <c r="I108" s="1">
@@ -10016,34 +9999,34 @@
       <c r="J108" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K108" s="15">
+      <c r="K108" s="1">
         <v>0.2</v>
       </c>
       <c r="L108" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M108" s="15">
+      <c r="M108" s="1">
         <v>26800</v>
       </c>
       <c r="N108" s="4">
         <v>500</v>
       </c>
-      <c r="O108" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P108" s="15" t="s">
+      <c r="O108" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P108" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q108" s="15">
+      <c r="Q108" s="1">
         <v>1E-3</v>
       </c>
-      <c r="R108" s="15">
-        <v>0</v>
-      </c>
-      <c r="S108" s="15">
-        <v>0</v>
-      </c>
-      <c r="T108" s="15">
+      <c r="R108" s="1">
+        <v>0</v>
+      </c>
+      <c r="S108" s="1">
+        <v>0</v>
+      </c>
+      <c r="T108" s="1">
         <v>512</v>
       </c>
       <c r="U108" s="2">
@@ -10073,22 +10056,22 @@
       <c r="B109" s="1">
         <v>2</v>
       </c>
-      <c r="C109" s="15">
+      <c r="C109" s="1">
         <v>50</v>
       </c>
-      <c r="D109" s="4" t="s">
+      <c r="D109" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E109" s="4" t="s">
+      <c r="E109" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F109" s="15">
+      <c r="F109" s="1">
         <v>2</v>
       </c>
       <c r="G109" s="1">
         <v>0</v>
       </c>
-      <c r="H109" s="15">
+      <c r="H109" s="1">
         <v>0</v>
       </c>
       <c r="I109" s="1">
@@ -10097,34 +10080,34 @@
       <c r="J109" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K109" s="15">
+      <c r="K109" s="1">
         <v>0.2</v>
       </c>
       <c r="L109" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M109" s="15">
+      <c r="M109" s="1">
         <v>26800</v>
       </c>
-      <c r="N109" s="15">
+      <c r="N109" s="1">
         <v>500</v>
       </c>
-      <c r="O109" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="P109" s="15" t="s">
+      <c r="O109" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P109" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q109" s="15">
+      <c r="Q109" s="1">
         <v>1E-3</v>
       </c>
-      <c r="R109" s="15">
+      <c r="R109" s="1">
         <v>0</v>
       </c>
       <c r="S109" s="4">
         <v>0.5</v>
       </c>
-      <c r="T109" s="15">
+      <c r="T109" s="1">
         <v>512</v>
       </c>
       <c r="U109" s="2">
@@ -10136,7 +10119,7 @@
       <c r="W109" s="2">
         <v>335</v>
       </c>
-      <c r="X109" s="17">
+      <c r="X109" s="14">
         <v>0.9</v>
       </c>
       <c r="Y109" s="11" t="s">
@@ -10146,6 +10129,330 @@
       <c r="AA109" s="2" t="s">
         <v>134</v>
       </c>
+    </row>
+    <row r="110" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
+        <v>106</v>
+      </c>
+      <c r="B110" s="1">
+        <v>2</v>
+      </c>
+      <c r="C110" s="1">
+        <v>50</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F110" s="1">
+        <v>2</v>
+      </c>
+      <c r="G110" s="1">
+        <v>0</v>
+      </c>
+      <c r="H110" s="1">
+        <v>0</v>
+      </c>
+      <c r="I110" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K110" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L110" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M110" s="1">
+        <v>26800</v>
+      </c>
+      <c r="N110" s="1">
+        <v>500</v>
+      </c>
+      <c r="O110" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P110" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q110" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="R110" s="1">
+        <v>0</v>
+      </c>
+      <c r="S110" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T110" s="4">
+        <v>1024</v>
+      </c>
+      <c r="U110" s="2">
+        <v>91.89</v>
+      </c>
+      <c r="V110" s="2">
+        <v>76.77</v>
+      </c>
+      <c r="W110" s="2">
+        <v>328</v>
+      </c>
+      <c r="X110" s="7">
+        <v>0.9032</v>
+      </c>
+      <c r="Y110" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z110" s="1"/>
+      <c r="AA110" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="111" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
+        <v>107</v>
+      </c>
+      <c r="B111" s="1">
+        <v>2</v>
+      </c>
+      <c r="C111" s="1">
+        <v>50</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F111" s="1">
+        <v>2</v>
+      </c>
+      <c r="G111" s="1">
+        <v>0</v>
+      </c>
+      <c r="H111" s="1">
+        <v>0</v>
+      </c>
+      <c r="I111" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K111" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L111" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M111" s="1">
+        <v>26800</v>
+      </c>
+      <c r="N111" s="1">
+        <v>500</v>
+      </c>
+      <c r="O111" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P111" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q111" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="R111" s="1">
+        <v>0</v>
+      </c>
+      <c r="S111" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T111" s="4">
+        <v>2048</v>
+      </c>
+      <c r="U111" s="2">
+        <v>93.26</v>
+      </c>
+      <c r="V111" s="2">
+        <v>76.319999999999993</v>
+      </c>
+      <c r="W111" s="2">
+        <v>327</v>
+      </c>
+      <c r="X111" s="7">
+        <v>0.90090000000000003</v>
+      </c>
+      <c r="Y111" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z111" s="1"/>
+      <c r="AA111" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="112" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
+        <v>108</v>
+      </c>
+      <c r="B112" s="1">
+        <v>2</v>
+      </c>
+      <c r="C112" s="4">
+        <v>100</v>
+      </c>
+      <c r="D112" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F112" s="1">
+        <v>2</v>
+      </c>
+      <c r="G112" s="4">
+        <v>20</v>
+      </c>
+      <c r="H112" s="1">
+        <v>0</v>
+      </c>
+      <c r="I112" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J112" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K112" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L112" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M112" s="4">
+        <v>33900</v>
+      </c>
+      <c r="N112" s="1">
+        <v>500</v>
+      </c>
+      <c r="O112" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P112" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q112" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="R112" s="1">
+        <v>0</v>
+      </c>
+      <c r="S112" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T112" s="4">
+        <v>1024</v>
+      </c>
+      <c r="U112" s="2">
+        <v>93.19</v>
+      </c>
+      <c r="V112" s="2">
+        <v>74.38</v>
+      </c>
+      <c r="W112" s="2">
+        <v>420</v>
+      </c>
+      <c r="X112" s="7">
+        <v>0.87070000000000003</v>
+      </c>
+      <c r="Y112" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z112" s="1"/>
+      <c r="AA112" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="113" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
+        <v>109</v>
+      </c>
+      <c r="B113" s="1">
+        <v>2</v>
+      </c>
+      <c r="C113" s="4">
+        <v>200</v>
+      </c>
+      <c r="D113" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E113" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="F113" s="16">
+        <v>2</v>
+      </c>
+      <c r="G113" s="1">
+        <v>20</v>
+      </c>
+      <c r="H113" s="16">
+        <v>0</v>
+      </c>
+      <c r="I113" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K113" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M113" s="4">
+        <v>66400</v>
+      </c>
+      <c r="N113" s="16">
+        <v>500</v>
+      </c>
+      <c r="O113" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="P113" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q113" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="R113" s="16">
+        <v>0</v>
+      </c>
+      <c r="S113" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="T113" s="16">
+        <v>1024</v>
+      </c>
+      <c r="U113" s="2">
+        <v>88.17</v>
+      </c>
+      <c r="V113" s="2">
+        <v>70.290000000000006</v>
+      </c>
+      <c r="W113" s="2">
+        <v>804</v>
+      </c>
+      <c r="X113" s="7">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="Y113" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z113" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="AA113" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10153,16 +10460,16 @@
     <mergeCell ref="S1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="U2:U109">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
+  <conditionalFormatting sqref="U2:U113">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
iteration 3. relu experimentation, reverted to just summation for sequential aggregation.
</commit_message>
<xml_diff>
--- a/code/test results.xlsx
+++ b/code/test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73719973-0A2B-4900-9CE8-8A6D739A0FEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B01C44-07DA-4FD5-B2BB-BCEEFDA9F4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="142">
   <si>
     <t>test number</t>
   </si>
@@ -518,6 +518,16 @@
   <si>
     <t>changed code to be more memory efficient
 should NOT cause memory leaks*</t>
+  </si>
+  <si>
+    <t>introduction of new model. Introduces
+ReLU after each linear layer</t>
+  </si>
+  <si>
+    <t>best_model_069.pth</t>
+  </si>
+  <si>
+    <t>best_model_070.pth</t>
   </si>
 </sst>
 </file>
@@ -652,7 +662,28 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="38">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -970,39 +1001,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA113" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
-  <autoFilter ref="A2:AA113" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA115" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+  <autoFilter ref="A2:AA115" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:AA76">
     <sortCondition ref="C2:C80"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="32"/>
-    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="31"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="30"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="29"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="27"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="26"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="25"/>
-    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="23"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="22"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="20"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="18"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="17"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="16"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="15"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="14"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="13"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="12"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="11"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="10"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="9"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="8"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="7"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="6"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="35"/>
+    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="34"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="33"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="32"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="28"/>
+    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="27"/>
+    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1305,10 +1336,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:AA113"/>
+  <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G85" workbookViewId="0">
-      <selection activeCell="M119" sqref="M119"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8602,7 +8633,7 @@
       <c r="B91" s="1">
         <v>1</v>
       </c>
-      <c r="C91" s="1">
+      <c r="C91" s="4">
         <v>50</v>
       </c>
       <c r="D91" s="1" t="s">
@@ -9879,7 +9910,7 @@
       <c r="X106" s="7">
         <v>0.80389999999999995</v>
       </c>
-      <c r="Y106" s="11" t="s">
+      <c r="Y106" s="10" t="s">
         <v>65</v>
       </c>
       <c r="Z106" s="1"/>
@@ -10383,19 +10414,19 @@
       <c r="C113" s="4">
         <v>200</v>
       </c>
-      <c r="D113" s="16" t="s">
+      <c r="D113" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="E113" s="16" t="s">
+      <c r="E113" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="F113" s="16">
+      <c r="F113" s="1">
         <v>2</v>
       </c>
       <c r="G113" s="1">
         <v>20</v>
       </c>
-      <c r="H113" s="16">
+      <c r="H113" s="1">
         <v>0</v>
       </c>
       <c r="I113" s="1">
@@ -10404,7 +10435,7 @@
       <c r="J113" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K113" s="16">
+      <c r="K113" s="1">
         <v>0.2</v>
       </c>
       <c r="L113" s="1" t="s">
@@ -10413,25 +10444,25 @@
       <c r="M113" s="4">
         <v>66400</v>
       </c>
-      <c r="N113" s="16">
+      <c r="N113" s="1">
         <v>500</v>
       </c>
-      <c r="O113" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="P113" s="16" t="s">
+      <c r="O113" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P113" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="Q113" s="16">
+      <c r="Q113" s="1">
         <v>1E-3</v>
       </c>
-      <c r="R113" s="16">
-        <v>0</v>
-      </c>
-      <c r="S113" s="16">
+      <c r="R113" s="1">
+        <v>0</v>
+      </c>
+      <c r="S113" s="1">
         <v>0.5</v>
       </c>
-      <c r="T113" s="16">
+      <c r="T113" s="1">
         <v>1024</v>
       </c>
       <c r="U113" s="2">
@@ -10453,6 +10484,172 @@
         <v>138</v>
       </c>
       <c r="AA113" s="2"/>
+    </row>
+    <row r="114" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
+        <v>110</v>
+      </c>
+      <c r="B114" s="1">
+        <v>2</v>
+      </c>
+      <c r="C114" s="16">
+        <v>50</v>
+      </c>
+      <c r="D114" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F114" s="1">
+        <v>2</v>
+      </c>
+      <c r="G114" s="4">
+        <v>0</v>
+      </c>
+      <c r="H114" s="1">
+        <v>0</v>
+      </c>
+      <c r="I114" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J114" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K114" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L114" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M114" s="4">
+        <v>26800</v>
+      </c>
+      <c r="N114" s="4">
+        <v>100</v>
+      </c>
+      <c r="O114" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P114" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q114" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="R114" s="1">
+        <v>0</v>
+      </c>
+      <c r="S114" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T114" s="1">
+        <v>1024</v>
+      </c>
+      <c r="U114" s="2">
+        <v>86.3</v>
+      </c>
+      <c r="V114" s="2">
+        <v>72.430000000000007</v>
+      </c>
+      <c r="W114" s="2">
+        <v>2640</v>
+      </c>
+      <c r="X114" s="7">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="Y114" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z114" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AA114" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="115" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="A115" s="1">
+        <v>111</v>
+      </c>
+      <c r="B115" s="4">
+        <v>3</v>
+      </c>
+      <c r="C115" s="16">
+        <v>50</v>
+      </c>
+      <c r="D115" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F115" s="1">
+        <v>2</v>
+      </c>
+      <c r="G115" s="1">
+        <v>0</v>
+      </c>
+      <c r="H115" s="1">
+        <v>0</v>
+      </c>
+      <c r="I115" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="J115" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K115" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="L115" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M115" s="16">
+        <v>26800</v>
+      </c>
+      <c r="N115" s="4">
+        <v>50</v>
+      </c>
+      <c r="O115" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P115" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q115" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="R115" s="1">
+        <v>0</v>
+      </c>
+      <c r="S115" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="T115" s="1">
+        <v>1024</v>
+      </c>
+      <c r="U115" s="2">
+        <v>86.81</v>
+      </c>
+      <c r="V115" s="2">
+        <v>73.06</v>
+      </c>
+      <c r="W115" s="2">
+        <v>4505</v>
+      </c>
+      <c r="X115" s="7">
+        <v>0.88429999999999997</v>
+      </c>
+      <c r="Y115" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z115" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="AA115" s="2" t="s">
+        <v>141</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -10460,16 +10657,16 @@
     <mergeCell ref="S1:V1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="U2:U113">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="between">
+  <conditionalFormatting sqref="U2:U115">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
extra comment for iteration 2
</commit_message>
<xml_diff>
--- a/code/test results.xlsx
+++ b/code/test results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0B01C44-07DA-4FD5-B2BB-BCEEFDA9F4DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A65D9999-1445-46DE-960A-DC31E1C8CAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1128" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="143">
   <si>
     <t>test number</t>
   </si>
@@ -528,6 +528,11 @@
   </si>
   <si>
     <t>best_model_070.pth</t>
+  </si>
+  <si>
+    <t>new model. Batch normalisation applied
++ other features (check diff between models
+in model_iterations folder)</t>
   </si>
 </sst>
 </file>
@@ -608,7 +613,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -655,56 +660,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF630D"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill>
@@ -1001,39 +961,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA115" totalsRowShown="0" headerRowDxfId="37" dataDxfId="36">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AA115" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
   <autoFilter ref="A2:AA115" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:AA76">
     <sortCondition ref="C2:C80"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="35"/>
-    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="34"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="33"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="32"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="31"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="30"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="28"/>
-    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="27"/>
-    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="26"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="29"/>
+    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="27"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="26"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="24"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="22"/>
+    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="21"/>
+    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="19"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="17"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="16"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="14"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="13"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="12"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="11"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="10"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="9"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="8"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="7"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="6"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="5"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="4"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1338,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
   <dimension ref="A1:AA115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="I82" workbookViewId="0">
+      <selection activeCell="Q89" sqref="Q89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9112,7 +9072,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="97" spans="1:27" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:27" ht="45" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>93</v>
       </c>
@@ -9188,7 +9148,9 @@
       <c r="Y97" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Z97" s="1"/>
+      <c r="Z97" s="6" t="s">
+        <v>142</v>
+      </c>
       <c r="AA97" s="2" t="s">
         <v>118</v>
       </c>
@@ -10492,7 +10454,7 @@
       <c r="B114" s="1">
         <v>2</v>
       </c>
-      <c r="C114" s="16">
+      <c r="C114" s="1">
         <v>50</v>
       </c>
       <c r="D114" s="1" t="s">
@@ -10575,7 +10537,7 @@
       <c r="B115" s="4">
         <v>3</v>
       </c>
-      <c r="C115" s="16">
+      <c r="C115" s="1">
         <v>50</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -10605,7 +10567,7 @@
       <c r="L115" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="M115" s="16">
+      <c r="M115" s="1">
         <v>26800</v>
       </c>
       <c r="N115" s="4">
@@ -10658,15 +10620,15 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="U2:U115">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
extra tests and aggregation functions experimented
</commit_message>
<xml_diff>
--- a/code/test results.xlsx
+++ b/code/test results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bradl\Desktop\uni\final-project\code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D23DCD9-98D0-43BF-BF62-0D7966434EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E51A877-9739-4720-9796-552F3352C7C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5280" windowWidth="29040" windowHeight="15840" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{8A721CCB-E596-4063-BEBF-8402B06F69EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1146" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1300" uniqueCount="150">
   <si>
     <t>test number</t>
   </si>
@@ -539,6 +539,24 @@
   </si>
   <si>
     <t>sampling rate (hz)</t>
+  </si>
+  <si>
+    <t>above 2 tests but on SCIAMA</t>
+  </si>
+  <si>
+    <t>62 .18%</t>
+  </si>
+  <si>
+    <t>scaled mel spectrogram values to be
+between 0-80 instead of all over the place</t>
+  </si>
+  <si>
+    <t>mean and variance threshold reintroduced,
+new settings in place</t>
+  </si>
+  <si>
+    <t>instead of removing silence, make it its own
+class and train the model on it.</t>
   </si>
 </sst>
 </file>
@@ -619,7 +637,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -666,11 +684,56 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF630D"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -970,40 +1033,40 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AB117" totalsRowShown="0" headerRowDxfId="32" dataDxfId="31">
-  <autoFilter ref="A2:AB117" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}" name="Table1" displayName="Table1" ref="A2:AB140" totalsRowShown="0" headerRowDxfId="38" dataDxfId="37">
+  <autoFilter ref="A2:AB140" xr:uid="{BDC20197-0D11-4F96-98C6-561676E67A6E}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A35:AB76">
     <sortCondition ref="C2:C80"/>
   </sortState>
   <tableColumns count="28">
-    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="30"/>
-    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="28"/>
-    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="27"/>
-    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="26"/>
-    <tableColumn id="28" xr3:uid="{8B631FC7-380A-498A-87D1-A5A5CDE1B184}" name="sampling rate (hz)" dataDxfId="25"/>
-    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="24"/>
-    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="23"/>
-    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="22"/>
-    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="21"/>
-    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="19"/>
-    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="17"/>
-    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="15"/>
-    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="14"/>
-    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="13"/>
-    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="12"/>
-    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="11"/>
-    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="10"/>
-    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="9"/>
-    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="8"/>
-    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="7"/>
-    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="6"/>
-    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="5"/>
-    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="4"/>
-    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3318AD16-53B6-4688-8184-DCAE4D7989CC}" name="test number" dataDxfId="36"/>
+    <tableColumn id="26" xr3:uid="{36FCCC2D-6AA9-4D59-9607-CFE4E77F428F}" name="model iteration" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{6162A6E9-56C2-4DFE-8497-138E33277B23}" name="folders" dataDxfId="34"/>
+    <tableColumn id="24" xr3:uid="{84500DC1-61E5-441B-9BB7-98403DAEDDA3}" name="single or multi label" dataDxfId="33"/>
+    <tableColumn id="23" xr3:uid="{D53465F0-58BB-492A-A264-D9F6F9AD3C77}" name="file rating threshold" dataDxfId="32"/>
+    <tableColumn id="28" xr3:uid="{8B631FC7-380A-498A-87D1-A5A5CDE1B184}" name="sampling rate (hz)" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{455DD90A-7B3B-4AE3-B08F-EF626809FA12}" name="sound length (secs)" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{BE562B7A-09E8-48B6-87F1-F9358A9B6D5B}" name="files per folder threshold" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{E3C34C6B-84EB-4093-B2F3-6A3FEA8E014C}" name="sound clips per file threshold" dataDxfId="28"/>
+    <tableColumn id="27" xr3:uid="{191D39FF-C4F8-4DBA-B0D0-9163B957A029}" name="variance threshold" dataDxfId="27"/>
+    <tableColumn id="25" xr3:uid="{E5B8107D-0DF4-4EA1-ADD9-375779D45EF4}" name="mean db threshold" dataDxfId="26"/>
+    <tableColumn id="19" xr3:uid="{864FBBD1-F7F9-4946-B210-D69AFB5835DC}" name="test size" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{2B2C8707-3EBF-4F34-8873-79CDF32B12F6}" name="sampling" dataDxfId="24"/>
+    <tableColumn id="5" xr3:uid="{F22E151A-20C9-4BD4-9330-289A7FFEA185}" name="sound clips" dataDxfId="23"/>
+    <tableColumn id="18" xr3:uid="{5798ECBB-EF37-49E5-8484-9B35165F789E}" name="epochs" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{FCBAD803-5AC6-4170-96E5-CDADD42AAFE6}" name="loss function" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{28105F38-9933-41DD-903D-59C6CB55BAC1}" name="optimizer" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{EB347492-3ECD-4D09-9D3B-70F1B3841DE0}" name="learning rate" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{E8435981-3E1D-4BD4-B5A5-B92A95E47B32}" name="momentum" dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{6CFBA716-45FB-401C-A304-C38379448F6E}" name="dropout rate" dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{696423D6-C6E9-46A6-845B-0AF07B48592B}" name="batch size" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{7FD1D4E4-3292-4AA1-9BCC-2B94A81E0391}" name="training accuracy %" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{8EE7A374-9D10-4C25-9169-E97C46453BAF}" name="testing accuracy %" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{E1A45F5D-7C07-400E-8A62-BFF33A480A4C}" name="gpu train time (secs)" dataDxfId="13"/>
+    <tableColumn id="20" xr3:uid="{B80BC466-5D5A-48F1-9455-63991D7EF174}" name="top-5 accuracy" dataDxfId="12"/>
+    <tableColumn id="21" xr3:uid="{E7EF58AA-8977-49AA-AE41-D484359C41A5}" name="tested on?" dataDxfId="11"/>
+    <tableColumn id="15" xr3:uid="{26BF47AC-1BE1-47B7-86FA-94CD5B2EA529}" name="other changes" dataDxfId="10"/>
+    <tableColumn id="17" xr3:uid="{3D30E15F-1B0A-4446-9BD7-F4008384352E}" name="best iteration model file path" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1306,10 +1369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FCC9065-8250-489C-BD55-B74D78928912}">
-  <dimension ref="A1:AB117"/>
+  <dimension ref="A1:AB140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="X118" sqref="X118"/>
+    <sheetView tabSelected="1" topLeftCell="J106" workbookViewId="0">
+      <selection activeCell="S130" sqref="S130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9900,7 +9963,7 @@
       <c r="J103" s="1">
         <v>0.2</v>
       </c>
-      <c r="K103" s="1">
+      <c r="K103" s="4">
         <v>5</v>
       </c>
       <c r="L103" s="1">
@@ -10070,7 +10133,7 @@
       <c r="J105" s="1">
         <v>0.2</v>
       </c>
-      <c r="K105" s="1" t="s">
+      <c r="K105" s="4" t="s">
         <v>29</v>
       </c>
       <c r="L105" s="1">
@@ -11134,6 +11197,1900 @@
         <v>143</v>
       </c>
       <c r="AB117" s="2"/>
+    </row>
+    <row r="118" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>114</v>
+      </c>
+      <c r="B118" s="1">
+        <v>3</v>
+      </c>
+      <c r="C118" s="1">
+        <v>50</v>
+      </c>
+      <c r="D118" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E118" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F118" s="4">
+        <v>32000</v>
+      </c>
+      <c r="G118" s="1">
+        <v>2</v>
+      </c>
+      <c r="H118" s="1">
+        <v>0</v>
+      </c>
+      <c r="I118" s="1">
+        <v>0</v>
+      </c>
+      <c r="J118" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L118" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M118" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N118" s="4">
+        <v>26800</v>
+      </c>
+      <c r="O118" s="4">
+        <v>500</v>
+      </c>
+      <c r="P118" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q118" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R118" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S118" s="1">
+        <v>0</v>
+      </c>
+      <c r="T118" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U118" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V118" s="2">
+        <v>83.58</v>
+      </c>
+      <c r="W118" s="2">
+        <v>72.78</v>
+      </c>
+      <c r="X118" s="2">
+        <v>351</v>
+      </c>
+      <c r="Y118" s="7">
+        <v>0.77949999999999997</v>
+      </c>
+      <c r="Z118" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA118" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AB118" s="2"/>
+    </row>
+    <row r="119" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A119" s="1">
+        <v>115</v>
+      </c>
+      <c r="B119" s="1">
+        <v>3</v>
+      </c>
+      <c r="C119" s="1">
+        <v>50</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E119" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F119" s="4">
+        <v>16000</v>
+      </c>
+      <c r="G119" s="1">
+        <v>2</v>
+      </c>
+      <c r="H119" s="1">
+        <v>0</v>
+      </c>
+      <c r="I119" s="1">
+        <v>0</v>
+      </c>
+      <c r="J119" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L119" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M119" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N119" s="4">
+        <v>27050</v>
+      </c>
+      <c r="O119" s="1">
+        <v>500</v>
+      </c>
+      <c r="P119" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q119" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R119" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S119" s="1">
+        <v>0</v>
+      </c>
+      <c r="T119" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U119" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V119" s="2">
+        <v>83.82</v>
+      </c>
+      <c r="W119" s="2">
+        <v>71.150000000000006</v>
+      </c>
+      <c r="X119" s="2">
+        <v>188</v>
+      </c>
+      <c r="Y119" s="7">
+        <v>0.79390000000000005</v>
+      </c>
+      <c r="Z119" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA119" s="1"/>
+      <c r="AB119" s="2"/>
+    </row>
+    <row r="120" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A120" s="1">
+        <v>116</v>
+      </c>
+      <c r="B120" s="1">
+        <v>3</v>
+      </c>
+      <c r="C120" s="4">
+        <v>200</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F120" s="1">
+        <v>16000</v>
+      </c>
+      <c r="G120" s="1">
+        <v>2</v>
+      </c>
+      <c r="H120" s="4">
+        <v>50</v>
+      </c>
+      <c r="I120" s="1">
+        <v>0</v>
+      </c>
+      <c r="J120" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L120" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M120" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N120" s="4">
+        <v>111200</v>
+      </c>
+      <c r="O120" s="1">
+        <v>500</v>
+      </c>
+      <c r="P120" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q120" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R120" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S120" s="1">
+        <v>0</v>
+      </c>
+      <c r="T120" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U120" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V120" s="2">
+        <v>69.67</v>
+      </c>
+      <c r="W120" s="2">
+        <v>56.53</v>
+      </c>
+      <c r="X120" s="2">
+        <v>746</v>
+      </c>
+      <c r="Y120" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="Z120" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA120" s="1"/>
+      <c r="AB120" s="2"/>
+    </row>
+    <row r="121" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A121" s="1">
+        <v>118</v>
+      </c>
+      <c r="B121" s="1">
+        <v>3</v>
+      </c>
+      <c r="C121" s="4">
+        <v>400</v>
+      </c>
+      <c r="D121" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F121" s="1">
+        <v>16000</v>
+      </c>
+      <c r="G121" s="1">
+        <v>2</v>
+      </c>
+      <c r="H121" s="1">
+        <v>50</v>
+      </c>
+      <c r="I121" s="1">
+        <v>0</v>
+      </c>
+      <c r="J121" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L121" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M121" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N121" s="4">
+        <v>228000</v>
+      </c>
+      <c r="O121" s="1">
+        <v>500</v>
+      </c>
+      <c r="P121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q121" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R121" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S121" s="1">
+        <v>0</v>
+      </c>
+      <c r="T121" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U121" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V121" s="2">
+        <v>58.46</v>
+      </c>
+      <c r="W121" s="2">
+        <v>46.62</v>
+      </c>
+      <c r="X121" s="2">
+        <v>1530</v>
+      </c>
+      <c r="Y121" s="7">
+        <v>0.51719999999999999</v>
+      </c>
+      <c r="Z121" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA121" s="1"/>
+      <c r="AB121" s="2"/>
+    </row>
+    <row r="122" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A122" s="1">
+        <v>119</v>
+      </c>
+      <c r="B122" s="1">
+        <v>3</v>
+      </c>
+      <c r="C122" s="4">
+        <v>50</v>
+      </c>
+      <c r="D122" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E122" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F122" s="4">
+        <v>32000</v>
+      </c>
+      <c r="G122" s="1">
+        <v>2</v>
+      </c>
+      <c r="H122" s="4">
+        <v>0</v>
+      </c>
+      <c r="I122" s="1">
+        <v>0</v>
+      </c>
+      <c r="J122" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L122" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M122" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N122" s="4">
+        <v>26800</v>
+      </c>
+      <c r="O122" s="1">
+        <v>500</v>
+      </c>
+      <c r="P122" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q122" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R122" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S122" s="1">
+        <v>0</v>
+      </c>
+      <c r="T122" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U122" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V122" s="2">
+        <v>82.43</v>
+      </c>
+      <c r="W122" s="2">
+        <v>71.62</v>
+      </c>
+      <c r="X122" s="2">
+        <v>342</v>
+      </c>
+      <c r="Y122" s="7">
+        <v>0.77370000000000005</v>
+      </c>
+      <c r="Z122" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA122" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AB122" s="2"/>
+    </row>
+    <row r="123" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A123" s="1">
+        <v>120</v>
+      </c>
+      <c r="B123" s="1">
+        <v>3</v>
+      </c>
+      <c r="C123" s="1">
+        <v>50</v>
+      </c>
+      <c r="D123" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E123" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F123" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G123" s="1">
+        <v>2</v>
+      </c>
+      <c r="H123" s="1">
+        <v>0</v>
+      </c>
+      <c r="I123" s="1">
+        <v>0</v>
+      </c>
+      <c r="J123" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L123" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M123" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N123" s="1">
+        <v>26800</v>
+      </c>
+      <c r="O123" s="1">
+        <v>500</v>
+      </c>
+      <c r="P123" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q123" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R123" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S123" s="1">
+        <v>0</v>
+      </c>
+      <c r="T123" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U123" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V123" s="2">
+        <v>83.55</v>
+      </c>
+      <c r="W123" s="2">
+        <v>71.959999999999994</v>
+      </c>
+      <c r="X123" s="2">
+        <v>340</v>
+      </c>
+      <c r="Y123" s="7">
+        <v>0.78149999999999997</v>
+      </c>
+      <c r="Z123" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA123" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="AB123" s="2"/>
+    </row>
+    <row r="124" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A124" s="1">
+        <v>121</v>
+      </c>
+      <c r="B124" s="1">
+        <v>3</v>
+      </c>
+      <c r="C124" s="1">
+        <v>50</v>
+      </c>
+      <c r="D124" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E124" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F124" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G124" s="1">
+        <v>2</v>
+      </c>
+      <c r="H124" s="1">
+        <v>0</v>
+      </c>
+      <c r="I124" s="1">
+        <v>0</v>
+      </c>
+      <c r="J124" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L124" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M124" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N124" s="1">
+        <v>26800</v>
+      </c>
+      <c r="O124" s="1">
+        <v>500</v>
+      </c>
+      <c r="P124" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R124" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S124" s="1">
+        <v>0</v>
+      </c>
+      <c r="T124" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="U124" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V124" s="2">
+        <v>85.33</v>
+      </c>
+      <c r="W124" s="2">
+        <v>71.81</v>
+      </c>
+      <c r="X124" s="2">
+        <v>340</v>
+      </c>
+      <c r="Y124" s="7">
+        <v>0.80989999999999995</v>
+      </c>
+      <c r="Z124" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA124" s="1"/>
+      <c r="AB124" s="2"/>
+    </row>
+    <row r="125" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A125" s="1">
+        <v>122</v>
+      </c>
+      <c r="B125" s="1">
+        <v>3</v>
+      </c>
+      <c r="C125" s="1">
+        <v>50</v>
+      </c>
+      <c r="D125" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E125" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F125" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G125" s="1">
+        <v>2</v>
+      </c>
+      <c r="H125" s="1">
+        <v>0</v>
+      </c>
+      <c r="I125" s="1">
+        <v>0</v>
+      </c>
+      <c r="J125" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L125" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M125" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N125" s="1">
+        <v>26800</v>
+      </c>
+      <c r="O125" s="1">
+        <v>500</v>
+      </c>
+      <c r="P125" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q125" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R125" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S125" s="1">
+        <v>0</v>
+      </c>
+      <c r="T125" s="4">
+        <v>0.3</v>
+      </c>
+      <c r="U125" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V125" s="2">
+        <v>89.9</v>
+      </c>
+      <c r="W125" s="2">
+        <v>75.760000000000005</v>
+      </c>
+      <c r="X125" s="2">
+        <v>337</v>
+      </c>
+      <c r="Y125" s="7">
+        <v>0.84589999999999999</v>
+      </c>
+      <c r="Z125" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA125" s="1"/>
+      <c r="AB125" s="2"/>
+    </row>
+    <row r="126" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A126" s="1">
+        <v>123</v>
+      </c>
+      <c r="B126" s="1">
+        <v>3</v>
+      </c>
+      <c r="C126" s="1">
+        <v>50</v>
+      </c>
+      <c r="D126" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E126" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F126" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G126" s="1">
+        <v>2</v>
+      </c>
+      <c r="H126" s="1">
+        <v>0</v>
+      </c>
+      <c r="I126" s="1">
+        <v>0</v>
+      </c>
+      <c r="J126" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L126" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M126" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N126" s="1">
+        <v>26800</v>
+      </c>
+      <c r="O126" s="1">
+        <v>500</v>
+      </c>
+      <c r="P126" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q126" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R126" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S126" s="1">
+        <v>0</v>
+      </c>
+      <c r="T126" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="U126" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V126" s="2">
+        <v>80.959999999999994</v>
+      </c>
+      <c r="W126" s="2">
+        <v>67.709999999999994</v>
+      </c>
+      <c r="X126" s="2">
+        <v>338</v>
+      </c>
+      <c r="Y126" s="7">
+        <v>0.73970000000000002</v>
+      </c>
+      <c r="Z126" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA126" s="1"/>
+      <c r="AB126" s="2"/>
+    </row>
+    <row r="127" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A127" s="1">
+        <v>124</v>
+      </c>
+      <c r="B127" s="1">
+        <v>3</v>
+      </c>
+      <c r="C127" s="1">
+        <v>50</v>
+      </c>
+      <c r="D127" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E127" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F127" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G127" s="1">
+        <v>2</v>
+      </c>
+      <c r="H127" s="1">
+        <v>0</v>
+      </c>
+      <c r="I127" s="1">
+        <v>0</v>
+      </c>
+      <c r="J127" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L127" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N127" s="1">
+        <v>26800</v>
+      </c>
+      <c r="O127" s="1">
+        <v>500</v>
+      </c>
+      <c r="P127" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q127" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R127" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S127" s="1">
+        <v>0</v>
+      </c>
+      <c r="T127" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="U127" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V127" s="2">
+        <v>86.84</v>
+      </c>
+      <c r="W127" s="2">
+        <v>70.819999999999993</v>
+      </c>
+      <c r="X127" s="2">
+        <v>338</v>
+      </c>
+      <c r="Y127" s="7">
+        <v>0.79239999999999999</v>
+      </c>
+      <c r="Z127" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA127" s="1"/>
+      <c r="AB127" s="2"/>
+    </row>
+    <row r="128" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A128" s="1">
+        <v>125</v>
+      </c>
+      <c r="B128" s="1">
+        <v>3</v>
+      </c>
+      <c r="C128" s="1">
+        <v>50</v>
+      </c>
+      <c r="D128" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E128" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F128" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G128" s="1">
+        <v>2</v>
+      </c>
+      <c r="H128" s="1">
+        <v>0</v>
+      </c>
+      <c r="I128" s="1">
+        <v>0</v>
+      </c>
+      <c r="J128" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L128" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N128" s="1">
+        <v>26800</v>
+      </c>
+      <c r="O128" s="1">
+        <v>500</v>
+      </c>
+      <c r="P128" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q128" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R128" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S128" s="1">
+        <v>0</v>
+      </c>
+      <c r="T128" s="4">
+        <v>0</v>
+      </c>
+      <c r="U128" s="1">
+        <v>1024</v>
+      </c>
+      <c r="V128" s="2">
+        <v>80.03</v>
+      </c>
+      <c r="W128" s="2">
+        <v>64.739999999999995</v>
+      </c>
+      <c r="X128" s="2">
+        <v>326</v>
+      </c>
+      <c r="Y128" s="7">
+        <v>0.72409999999999997</v>
+      </c>
+      <c r="Z128" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA128" s="1"/>
+      <c r="AB128" s="2"/>
+    </row>
+    <row r="129" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A129" s="1">
+        <v>126</v>
+      </c>
+      <c r="B129" s="1">
+        <v>3</v>
+      </c>
+      <c r="C129" s="1">
+        <v>50</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E129" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F129" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G129" s="1">
+        <v>2</v>
+      </c>
+      <c r="H129" s="1">
+        <v>0</v>
+      </c>
+      <c r="I129" s="1">
+        <v>0</v>
+      </c>
+      <c r="J129" s="4">
+        <v>1</v>
+      </c>
+      <c r="K129" s="4">
+        <v>5</v>
+      </c>
+      <c r="L129" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M129" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N129" s="4">
+        <v>25000</v>
+      </c>
+      <c r="O129" s="1">
+        <v>500</v>
+      </c>
+      <c r="P129" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q129" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R129" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S129" s="1">
+        <v>0</v>
+      </c>
+      <c r="T129" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="U129" s="4">
+        <v>1024</v>
+      </c>
+      <c r="V129" s="2">
+        <v>73.819999999999993</v>
+      </c>
+      <c r="W129" s="2">
+        <v>62.36</v>
+      </c>
+      <c r="X129" s="2">
+        <v>307</v>
+      </c>
+      <c r="Y129" s="7">
+        <v>0.67079999999999995</v>
+      </c>
+      <c r="Z129" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA129" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="AB129" s="2"/>
+    </row>
+    <row r="130" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A130" s="1">
+        <v>127</v>
+      </c>
+      <c r="B130" s="1">
+        <v>3</v>
+      </c>
+      <c r="C130" s="1">
+        <v>50</v>
+      </c>
+      <c r="D130" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E130" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F130" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G130" s="1">
+        <v>2</v>
+      </c>
+      <c r="H130" s="1">
+        <v>0</v>
+      </c>
+      <c r="I130" s="1">
+        <v>0</v>
+      </c>
+      <c r="J130" s="1">
+        <v>1</v>
+      </c>
+      <c r="K130" s="1">
+        <v>5</v>
+      </c>
+      <c r="L130" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M130" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N130" s="1">
+        <v>25000</v>
+      </c>
+      <c r="O130" s="1">
+        <v>500</v>
+      </c>
+      <c r="P130" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q130" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R130" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S130" s="1">
+        <v>0</v>
+      </c>
+      <c r="T130" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="U130" s="4">
+        <v>2048</v>
+      </c>
+      <c r="V130" s="2">
+        <v>85.7</v>
+      </c>
+      <c r="W130" s="2">
+        <v>71.260000000000005</v>
+      </c>
+      <c r="X130" s="2">
+        <v>299</v>
+      </c>
+      <c r="Y130" s="7">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="Z130" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA130" s="1"/>
+      <c r="AB130" s="2"/>
+    </row>
+    <row r="131" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A131" s="1">
+        <v>128</v>
+      </c>
+      <c r="B131" s="1">
+        <v>3</v>
+      </c>
+      <c r="C131" s="1">
+        <v>50</v>
+      </c>
+      <c r="D131" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E131" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F131" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G131" s="1">
+        <v>2</v>
+      </c>
+      <c r="H131" s="1">
+        <v>0</v>
+      </c>
+      <c r="I131" s="1">
+        <v>0</v>
+      </c>
+      <c r="J131" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="K131" s="1">
+        <v>5</v>
+      </c>
+      <c r="L131" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M131" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N131" s="4">
+        <v>26800</v>
+      </c>
+      <c r="O131" s="1">
+        <v>500</v>
+      </c>
+      <c r="P131" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q131" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R131" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S131" s="1">
+        <v>0</v>
+      </c>
+      <c r="T131" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U131" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V131" s="2">
+        <v>85.82</v>
+      </c>
+      <c r="W131" s="2">
+        <v>72.930000000000007</v>
+      </c>
+      <c r="X131" s="2">
+        <v>324</v>
+      </c>
+      <c r="Y131" s="7">
+        <v>0.8004</v>
+      </c>
+      <c r="Z131" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA131" s="1"/>
+      <c r="AB131" s="2"/>
+    </row>
+    <row r="132" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A132" s="1">
+        <v>129</v>
+      </c>
+      <c r="B132" s="1">
+        <v>3</v>
+      </c>
+      <c r="C132" s="1">
+        <v>50</v>
+      </c>
+      <c r="D132" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F132" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G132" s="1">
+        <v>2</v>
+      </c>
+      <c r="H132" s="4">
+        <v>20</v>
+      </c>
+      <c r="I132" s="1">
+        <v>0</v>
+      </c>
+      <c r="J132" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K132" s="1">
+        <v>5</v>
+      </c>
+      <c r="L132" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M132" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N132" s="4">
+        <v>17950</v>
+      </c>
+      <c r="O132" s="1">
+        <v>500</v>
+      </c>
+      <c r="P132" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q132" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R132" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S132" s="1">
+        <v>0</v>
+      </c>
+      <c r="T132" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U132" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V132" s="2">
+        <v>85.23</v>
+      </c>
+      <c r="W132" s="2">
+        <v>75.489999999999995</v>
+      </c>
+      <c r="X132" s="2">
+        <v>222</v>
+      </c>
+      <c r="Y132" s="7">
+        <v>0.80589999999999995</v>
+      </c>
+      <c r="Z132" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA132" s="1"/>
+      <c r="AB132" s="2"/>
+    </row>
+    <row r="133" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A133" s="1">
+        <v>130</v>
+      </c>
+      <c r="B133" s="1">
+        <v>3</v>
+      </c>
+      <c r="C133" s="1">
+        <v>50</v>
+      </c>
+      <c r="D133" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E133" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F133" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G133" s="1">
+        <v>2</v>
+      </c>
+      <c r="H133" s="4">
+        <v>0</v>
+      </c>
+      <c r="I133" s="1">
+        <v>0</v>
+      </c>
+      <c r="J133" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K133" s="4">
+        <v>10</v>
+      </c>
+      <c r="L133" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M133" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N133" s="4">
+        <v>26800</v>
+      </c>
+      <c r="O133" s="1">
+        <v>500</v>
+      </c>
+      <c r="P133" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q133" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R133" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S133" s="1">
+        <v>0</v>
+      </c>
+      <c r="T133" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U133" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V133" s="2">
+        <v>88.05</v>
+      </c>
+      <c r="W133" s="2">
+        <v>74.650000000000006</v>
+      </c>
+      <c r="X133" s="2">
+        <v>327</v>
+      </c>
+      <c r="Y133" s="7">
+        <v>0.82050000000000001</v>
+      </c>
+      <c r="Z133" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA133" s="1"/>
+      <c r="AB133" s="2"/>
+    </row>
+    <row r="134" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A134" s="1">
+        <v>131</v>
+      </c>
+      <c r="B134" s="1">
+        <v>3</v>
+      </c>
+      <c r="C134" s="1">
+        <v>50</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F134" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G134" s="1">
+        <v>2</v>
+      </c>
+      <c r="H134" s="4">
+        <v>20</v>
+      </c>
+      <c r="I134" s="1">
+        <v>0</v>
+      </c>
+      <c r="J134" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K134" s="1">
+        <v>10</v>
+      </c>
+      <c r="L134" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M134" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N134" s="4">
+        <v>17950</v>
+      </c>
+      <c r="O134" s="1">
+        <v>500</v>
+      </c>
+      <c r="P134" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q134" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R134" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S134" s="1">
+        <v>0</v>
+      </c>
+      <c r="T134" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U134" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V134" s="2">
+        <v>85.31</v>
+      </c>
+      <c r="W134" s="2">
+        <v>75.739999999999995</v>
+      </c>
+      <c r="X134" s="2">
+        <v>216</v>
+      </c>
+      <c r="Y134" s="7">
+        <v>0.81340000000000001</v>
+      </c>
+      <c r="Z134" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA134" s="1"/>
+      <c r="AB134" s="2"/>
+    </row>
+    <row r="135" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A135" s="1">
+        <v>132</v>
+      </c>
+      <c r="B135" s="1">
+        <v>3</v>
+      </c>
+      <c r="C135" s="1">
+        <v>50</v>
+      </c>
+      <c r="D135" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E135" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F135" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G135" s="1">
+        <v>2</v>
+      </c>
+      <c r="H135" s="4">
+        <v>0</v>
+      </c>
+      <c r="I135" s="1">
+        <v>0</v>
+      </c>
+      <c r="J135" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K135" s="4">
+        <v>15</v>
+      </c>
+      <c r="L135" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M135" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N135" s="4">
+        <v>26800</v>
+      </c>
+      <c r="O135" s="1">
+        <v>500</v>
+      </c>
+      <c r="P135" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q135" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R135" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S135" s="1">
+        <v>0</v>
+      </c>
+      <c r="T135" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U135" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V135" s="2">
+        <v>85.97</v>
+      </c>
+      <c r="W135" s="2">
+        <v>72.91</v>
+      </c>
+      <c r="X135" s="2">
+        <v>325</v>
+      </c>
+      <c r="Y135" s="7">
+        <v>0.80059999999999998</v>
+      </c>
+      <c r="Z135" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA135" s="1"/>
+      <c r="AB135" s="2"/>
+    </row>
+    <row r="136" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A136" s="1">
+        <v>133</v>
+      </c>
+      <c r="B136" s="1">
+        <v>3</v>
+      </c>
+      <c r="C136" s="1">
+        <v>50</v>
+      </c>
+      <c r="D136" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F136" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G136" s="1">
+        <v>2</v>
+      </c>
+      <c r="H136" s="4">
+        <v>20</v>
+      </c>
+      <c r="I136" s="1">
+        <v>0</v>
+      </c>
+      <c r="J136" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K136" s="1">
+        <v>15</v>
+      </c>
+      <c r="L136" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M136" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N136" s="4">
+        <v>17950</v>
+      </c>
+      <c r="O136" s="1">
+        <v>500</v>
+      </c>
+      <c r="P136" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q136" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R136" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S136" s="1">
+        <v>0</v>
+      </c>
+      <c r="T136" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U136" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V136" s="2">
+        <v>85.33</v>
+      </c>
+      <c r="W136" s="2">
+        <v>75.040000000000006</v>
+      </c>
+      <c r="X136" s="2">
+        <v>219</v>
+      </c>
+      <c r="Y136" s="7">
+        <v>0.81030000000000002</v>
+      </c>
+      <c r="Z136" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA136" s="1"/>
+      <c r="AB136" s="2"/>
+    </row>
+    <row r="137" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A137" s="1">
+        <v>134</v>
+      </c>
+      <c r="B137" s="1">
+        <v>3</v>
+      </c>
+      <c r="C137" s="1">
+        <v>50</v>
+      </c>
+      <c r="D137" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F137" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G137" s="1">
+        <v>2</v>
+      </c>
+      <c r="H137" s="4">
+        <v>0</v>
+      </c>
+      <c r="I137" s="1">
+        <v>0</v>
+      </c>
+      <c r="J137" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K137" s="4">
+        <v>20</v>
+      </c>
+      <c r="L137" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M137" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N137" s="4">
+        <v>26800</v>
+      </c>
+      <c r="O137" s="1">
+        <v>500</v>
+      </c>
+      <c r="P137" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q137" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R137" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S137" s="1">
+        <v>0</v>
+      </c>
+      <c r="T137" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U137" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V137" s="2">
+        <v>85.94</v>
+      </c>
+      <c r="W137" s="2">
+        <v>73.02</v>
+      </c>
+      <c r="X137" s="2">
+        <v>323</v>
+      </c>
+      <c r="Y137" s="7">
+        <v>0.79679999999999995</v>
+      </c>
+      <c r="Z137" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA137" s="1"/>
+      <c r="AB137" s="2"/>
+    </row>
+    <row r="138" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="1">
+        <v>135</v>
+      </c>
+      <c r="B138" s="1">
+        <v>3</v>
+      </c>
+      <c r="C138" s="1">
+        <v>50</v>
+      </c>
+      <c r="D138" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F138" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G138" s="1">
+        <v>2</v>
+      </c>
+      <c r="H138" s="4">
+        <v>20</v>
+      </c>
+      <c r="I138" s="1">
+        <v>0</v>
+      </c>
+      <c r="J138" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K138" s="1">
+        <v>20</v>
+      </c>
+      <c r="L138" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="M138" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N138" s="4">
+        <v>17950</v>
+      </c>
+      <c r="O138" s="1">
+        <v>500</v>
+      </c>
+      <c r="P138" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q138" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="R138" s="1">
+        <v>1E-3</v>
+      </c>
+      <c r="S138" s="1">
+        <v>0</v>
+      </c>
+      <c r="T138" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="U138" s="1">
+        <v>2048</v>
+      </c>
+      <c r="V138" s="2">
+        <v>85.12</v>
+      </c>
+      <c r="W138" s="2">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="X138" s="2">
+        <v>219</v>
+      </c>
+      <c r="Y138" s="7">
+        <v>0.80589999999999995</v>
+      </c>
+      <c r="Z138" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA138" s="1"/>
+      <c r="AB138" s="2"/>
+    </row>
+    <row r="139" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A139" s="1">
+        <v>136</v>
+      </c>
+      <c r="B139" s="1">
+        <v>3</v>
+      </c>
+      <c r="C139" s="16">
+        <v>50</v>
+      </c>
+      <c r="D139" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E139" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F139" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G139" s="1">
+        <v>2</v>
+      </c>
+      <c r="H139" s="16">
+        <v>20</v>
+      </c>
+      <c r="I139" s="16">
+        <v>0</v>
+      </c>
+      <c r="J139" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K139" s="4">
+        <v>5</v>
+      </c>
+      <c r="L139" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="M139" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N139" s="4">
+        <v>18513</v>
+      </c>
+      <c r="O139" s="16">
+        <v>500</v>
+      </c>
+      <c r="P139" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q139" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="R139" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="S139" s="16">
+        <v>0</v>
+      </c>
+      <c r="T139" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="U139" s="16">
+        <v>2048</v>
+      </c>
+      <c r="V139" s="2">
+        <v>91.94</v>
+      </c>
+      <c r="W139" s="2">
+        <v>78.069999999999993</v>
+      </c>
+      <c r="X139" s="2">
+        <v>255</v>
+      </c>
+      <c r="Y139" s="7">
+        <v>0.90010000000000001</v>
+      </c>
+      <c r="Z139" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA139" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AB139" s="2"/>
+    </row>
+    <row r="140" spans="1:28" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="1">
+        <v>137</v>
+      </c>
+      <c r="B140" s="1">
+        <v>3</v>
+      </c>
+      <c r="C140" s="16">
+        <v>50</v>
+      </c>
+      <c r="D140" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F140" s="1">
+        <v>32000</v>
+      </c>
+      <c r="G140" s="1">
+        <v>2</v>
+      </c>
+      <c r="H140" s="4">
+        <v>0</v>
+      </c>
+      <c r="I140" s="16">
+        <v>0</v>
+      </c>
+      <c r="J140" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="K140" s="16">
+        <v>5</v>
+      </c>
+      <c r="L140" s="16">
+        <v>0.2</v>
+      </c>
+      <c r="M140" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="N140" s="4">
+        <v>27693</v>
+      </c>
+      <c r="O140" s="16">
+        <v>500</v>
+      </c>
+      <c r="P140" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q140" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="R140" s="16">
+        <v>1E-3</v>
+      </c>
+      <c r="S140" s="16">
+        <v>0</v>
+      </c>
+      <c r="T140" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="U140" s="16">
+        <v>2048</v>
+      </c>
+      <c r="V140" s="2">
+        <v>85.91</v>
+      </c>
+      <c r="W140" s="2">
+        <v>71.31</v>
+      </c>
+      <c r="X140" s="2">
+        <v>369</v>
+      </c>
+      <c r="Y140" s="7">
+        <v>0.8337</v>
+      </c>
+      <c r="Z140" s="11"/>
+      <c r="AA140" s="1"/>
+      <c r="AB140" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -11141,16 +13098,16 @@
     <mergeCell ref="T1:W1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="V2:V117">
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="between">
+  <conditionalFormatting sqref="V2:V140">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="between">
       <formula>90</formula>
       <formula>99</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.01</formula>
       <formula>80</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>100</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>